<commit_message>
adding new rules and version 3.0.0
</commit_message>
<xml_diff>
--- a/test-dm-uae/src/main/resources/com/redhat/consulting/payment-review.xlsx
+++ b/test-dm-uae/src/main/resources/com/redhat/consulting/payment-review.xlsx
@@ -39,6 +39,7 @@
             <color rgb="FF000000"/>
             <rFont val="Times New Roman"/>
             <family val="1"/>
+            <charset val="1"/>
           </rPr>
           <t xml:space="preserve">A keyword of "Ruleset" means that this worksheet is a ruleset, and it has a name in the next cell across. In the following lines, we can have imports, or other ruleset directives if we need to ad them in future.
 </t>
@@ -49,6 +50,7 @@
             <color rgb="FF000000"/>
             <rFont val="Times New Roman"/>
             <family val="1"/>
+            <charset val="1"/>
           </rPr>
           <t xml:space="preserve">Perhaps this is not needed - ruleset name can be XLS name, and imports are not really needed most of the time.</t>
         </r>
@@ -63,6 +65,7 @@
             <color rgb="FF000000"/>
             <rFont val="Times New Roman"/>
             <family val="1"/>
+            <charset val="1"/>
           </rPr>
           <t xml:space="preserve">Look at me !! I tell you that I am the start of a rule table, and what parameters I require !
 </t>
@@ -73,6 +76,7 @@
             <color rgb="FF000000"/>
             <rFont val="Times New Roman"/>
             <family val="1"/>
+            <charset val="1"/>
           </rPr>
           <t xml:space="preserve">(and their types).
 The "RuleTable" keyword must appear on top of the first condition column.
@@ -90,6 +94,7 @@
             <color rgb="FF000000"/>
             <rFont val="Times New Roman"/>
             <family val="1"/>
+            <charset val="1"/>
           </rPr>
           <t xml:space="preserve">Look at me !!
 </t>
@@ -100,6 +105,7 @@
             <color rgb="FF000000"/>
             <rFont val="Times New Roman"/>
             <family val="1"/>
+            <charset val="1"/>
           </rPr>
           <t xml:space="preserve">I tell you that I am a condition colmn. The next row down has the rule "template" and the row below that is a comment. After that, it is all rule data until an empty line !
 Note that if there is no data in a row, then this condition does not apply. 
@@ -146,7 +152,7 @@
 insert($param);</t>
   </si>
   <si>
-    <t xml:space="preserve">Person Rules</t>
+    <t xml:space="preserve">Payment Rules</t>
   </si>
   <si>
     <t xml:space="preserve">Name</t>
@@ -213,6 +219,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -233,6 +240,7 @@
       <sz val="7"/>
       <name val="Tahoma"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -240,12 +248,14 @@
       <color rgb="FFFFFFFF"/>
       <name val="Tahoma"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="7"/>
       <color rgb="FFFFFFFF"/>
       <name val="Tahoma"/>
       <family val="0"/>
+      <charset val="1"/>
     </font>
     <font>
       <u val="single"/>
@@ -253,18 +263,21 @@
       <color rgb="FF0000D4"/>
       <name val="Arial"/>
       <family val="0"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
       <sz val="10"/>
       <name val="Courier New"/>
       <family val="3"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
       <sz val="7"/>
       <name val="Tahoma"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -272,6 +285,7 @@
       <color rgb="FF000000"/>
       <name val="Tahoma"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -279,12 +293,14 @@
       <color rgb="FF000000"/>
       <name val="Times New Roman"/>
       <family val="1"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="8"/>
       <color rgb="FF000000"/>
       <name val="Times New Roman"/>
       <family val="1"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="8">
@@ -441,9 +457,11 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="32">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -520,10 +538,6 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="165" fontId="9" fillId="3" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -569,10 +583,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="9" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -663,14 +673,14 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="200" zoomScaleNormal="200" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="2700" topLeftCell="A1" activePane="bottomLeft" state="split"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="D8" activeCellId="0" sqref="D8"/>
+      <selection pane="bottomLeft" activeCell="D7" activeCellId="0" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11" zeroHeight="false" outlineLevelRow="1" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="23.8"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="16.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="27.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="27.31"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="18.47"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="2" width="19.97"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="18.8"/>
@@ -678,8 +688,8 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="15.48"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="16.64"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="17.47"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="257" min="11" style="1" width="9.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="258" style="0" width="9.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="257" min="11" style="1" width="9.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="258" style="0" width="9.13"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -746,7 +756,7 @@
       <c r="IS6" s="0"/>
       <c r="IU6" s="0"/>
     </row>
-    <row r="7" s="19" customFormat="true" ht="11" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
+    <row r="7" s="1" customFormat="true" ht="11" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
       <c r="A7" s="16"/>
       <c r="B7" s="17" t="s">
         <v>6</v>
@@ -755,23 +765,23 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" s="23" customFormat="true" ht="28.85" hidden="false" customHeight="true" outlineLevel="1" collapsed="false">
-      <c r="A8" s="20"/>
-      <c r="B8" s="21" t="s">
+    <row r="8" s="22" customFormat="true" ht="28.85" hidden="false" customHeight="true" outlineLevel="1" collapsed="false">
+      <c r="A8" s="19"/>
+      <c r="B8" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="C8" s="22" t="s">
+      <c r="C8" s="21" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="28.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="24" t="s">
+      <c r="A9" s="23" t="s">
         <v>10</v>
       </c>
-      <c r="B9" s="25" t="s">
+      <c r="B9" s="24" t="s">
         <v>11</v>
       </c>
-      <c r="C9" s="26" t="s">
+      <c r="C9" s="25" t="s">
         <v>12</v>
       </c>
       <c r="E9" s="1"/>
@@ -779,13 +789,13 @@
       <c r="IS9" s="0"/>
     </row>
     <row r="10" customFormat="false" ht="12.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A10" s="27" t="s">
+      <c r="A10" s="26" t="s">
         <v>13</v>
       </c>
-      <c r="B10" s="28" t="s">
+      <c r="B10" s="27" t="s">
         <v>14</v>
       </c>
-      <c r="C10" s="29" t="s">
+      <c r="C10" s="28" t="s">
         <v>15</v>
       </c>
       <c r="E10" s="1"/>
@@ -793,13 +803,13 @@
       <c r="IS10" s="0"/>
     </row>
     <row r="11" customFormat="false" ht="12.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A11" s="27" t="s">
+      <c r="A11" s="26" t="s">
         <v>16</v>
       </c>
-      <c r="B11" s="28" t="s">
+      <c r="B11" s="27" t="s">
         <v>17</v>
       </c>
-      <c r="C11" s="29" t="s">
+      <c r="C11" s="28" t="s">
         <v>18</v>
       </c>
       <c r="E11" s="1"/>
@@ -807,9 +817,9 @@
       <c r="IS11" s="0"/>
     </row>
     <row r="12" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A12" s="30"/>
-      <c r="B12" s="31"/>
-      <c r="C12" s="29"/>
+      <c r="A12" s="29"/>
+      <c r="B12" s="30"/>
+      <c r="C12" s="28"/>
       <c r="E12" s="1"/>
       <c r="IR12" s="0"/>
       <c r="IS12" s="0"/>
@@ -846,7 +856,7 @@
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="17.97"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="8.81"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="17.31"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="17.32"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="8.81"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="16.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="6" style="0" width="8.81"/>
@@ -864,35 +874,35 @@
       </c>
     </row>
     <row r="5" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="32" t="s">
+      <c r="A5" s="31" t="s">
         <v>22</v>
       </c>
-      <c r="C5" s="32" t="s">
+      <c r="C5" s="31" t="s">
         <v>23</v>
       </c>
-      <c r="E5" s="32" t="s">
+      <c r="E5" s="31" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="33" t="s">
+      <c r="A6" s="31" t="s">
         <v>24</v>
       </c>
-      <c r="C6" s="32" t="s">
+      <c r="C6" s="31" t="s">
         <v>25</v>
       </c>
-      <c r="E6" s="32" t="s">
+      <c r="E6" s="31" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="32" t="s">
+      <c r="A7" s="31" t="s">
         <v>26</v>
       </c>
-      <c r="C7" s="32" t="s">
+      <c r="C7" s="31" t="s">
         <v>27</v>
       </c>
-      <c r="E7" s="32" t="s">
+      <c r="E7" s="31" t="s">
         <v>27</v>
       </c>
     </row>

</xml_diff>